<commit_message>
end of day update
</commit_message>
<xml_diff>
--- a/documents/DatabaseSchema.xlsx
+++ b/documents/DatabaseSchema.xlsx
@@ -811,12 +811,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1207,12 +1208,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>59</v>
@@ -1227,7 +1228,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -1247,7 +1248,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1493,7 +1494,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -1515,7 +1516,7 @@
       </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1537,7 +1538,7 @@
       </c>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -1559,7 +1560,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -1581,7 +1582,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -1624,7 +1625,7 @@
       </c>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -1644,7 +1645,7 @@
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -1664,7 +1665,7 @@
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -1684,7 +1685,7 @@
       </c>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1704,7 +1705,7 @@
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1726,7 +1727,7 @@
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
@@ -1748,7 +1749,7 @@
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>3</v>
       </c>
@@ -1770,7 +1771,7 @@
       </c>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>3</v>
       </c>
@@ -1792,7 +1793,7 @@
       </c>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +1815,7 @@
       </c>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>3</v>
       </c>
@@ -1836,7 +1837,7 @@
       </c>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>3</v>
       </c>
@@ -1858,7 +1859,7 @@
       </c>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>3</v>
       </c>
@@ -1880,7 +1881,7 @@
       </c>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>3</v>
       </c>
@@ -1902,7 +1903,7 @@
       </c>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
@@ -1922,7 +1923,7 @@
       </c>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>3</v>
       </c>
@@ -1942,7 +1943,7 @@
       </c>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>3</v>
       </c>
@@ -1962,7 +1963,7 @@
       </c>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>3</v>
       </c>
@@ -1982,7 +1983,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
@@ -2002,7 +2003,7 @@
       </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>3</v>
       </c>
@@ -2022,7 +2023,7 @@
       </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
@@ -2042,7 +2043,7 @@
       </c>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>3</v>
       </c>
@@ -2062,7 +2063,7 @@
       </c>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
@@ -2082,7 +2083,7 @@
       </c>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>3</v>
       </c>
@@ -2102,7 +2103,7 @@
       </c>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
@@ -2122,7 +2123,7 @@
       </c>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>3</v>
       </c>
@@ -2142,7 +2143,7 @@
       </c>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>3</v>
       </c>
@@ -2162,7 +2163,7 @@
       </c>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>3</v>
       </c>
@@ -2182,7 +2183,7 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>3</v>
       </c>
@@ -2367,7 +2368,7 @@
   <autoFilter ref="A1:G84">
     <filterColumn colId="0">
       <filters>
-        <filter val="Products"/>
+        <filter val="IPG"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>